<commit_message>
Intermediate updates to notebooks and new templates
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/ecuador/model_input_variables_ecuador_ip_calibrated.xlsx
+++ b/ref/ingestion/calibrated/ecuador/model_input_variables_ecuador_ip_calibrated.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="161">
   <si>
     <t>subsector</t>
   </si>
@@ -495,6 +495,9 @@
   <si>
     <t>vol_ippu_wood_m3_ww_per_tonne_production</t>
   </si>
+  <si>
+    <t>inf</t>
+  </si>
 </sst>
 </file>
 
@@ -1252,112 +1255,112 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="O4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="Q4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="R4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="S4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="U4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="V4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="W4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="X4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="Y4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="Z4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AA4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AB4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AC4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AD4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AE4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AF4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AG4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AH4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AI4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AJ4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AK4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AL4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AM4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AN4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AO4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AP4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AQ4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AR4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
       <c r="AS4">
-        <v>0.982214253</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:45">
@@ -1374,112 +1377,112 @@
         <v>1</v>
       </c>
       <c r="J5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="L5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="N5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="O5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="P5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="Q5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="R5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="S5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="T5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="U5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="V5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="W5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="X5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="Y5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="Z5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AA5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AB5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AC5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AD5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AE5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AF5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AG5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AH5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AI5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AJ5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AK5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AL5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AM5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AN5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AO5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AP5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AQ5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AR5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
       <c r="AS5">
-        <v>0.998873831</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:45">
@@ -1496,112 +1499,112 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="N6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="O6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="P6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="S6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="T6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="U6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="V6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="W6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="X6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="Y6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="Z6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AA6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AB6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AC6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AD6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AE6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AF6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AG6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AH6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AI6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AJ6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AK6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AL6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AM6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AN6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AO6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AP6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AQ6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AR6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
       <c r="AS6">
-        <v>1.017143149</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:45">
@@ -1618,112 +1621,112 @@
         <v>1</v>
       </c>
       <c r="J7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="K7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="L7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="N7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="O7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="P7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="Q7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="R7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="S7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="T7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="U7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="V7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="W7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="X7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="Y7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="Z7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AA7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AB7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AC7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AD7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AE7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AF7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AG7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AH7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AI7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AJ7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AK7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AL7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AM7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AN7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AO7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AP7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AQ7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AR7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
       <c r="AS7">
-        <v>1.021467454</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:45">
@@ -1740,112 +1743,112 @@
         <v>1</v>
       </c>
       <c r="J8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="K8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="L8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="M8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="N8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="O8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="P8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="Q8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="R8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="S8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="T8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="U8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="V8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="W8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="X8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="Y8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="Z8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AA8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AB8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AC8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AD8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AE8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AF8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AG8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AH8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AI8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AJ8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AK8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AL8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AM8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AN8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AO8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AP8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AQ8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AR8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
       <c r="AS8">
-        <v>0.973839233</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:45">
@@ -1862,112 +1865,112 @@
         <v>1</v>
       </c>
       <c r="J9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="L9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="M9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="N9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="O9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="P9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="Q9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="R9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="S9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="T9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="U9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="V9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="W9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="X9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="Y9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="Z9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AA9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AB9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AC9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AD9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AE9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AF9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AG9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AH9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AI9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AJ9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AK9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AL9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AM9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AN9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AO9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AP9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AQ9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AR9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
       <c r="AS9">
-        <v>1.020594953</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:45">
@@ -1984,112 +1987,112 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="K10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="L10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="M10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="N10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="O10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="P10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="Q10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="R10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="S10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="T10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="U10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="V10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="W10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="X10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="Y10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="Z10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AA10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AB10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AC10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AD10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AE10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AF10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AG10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AH10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AI10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AJ10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AK10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AL10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AM10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AN10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AO10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AP10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AQ10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AR10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
       <c r="AS10">
-        <v>0.974084233</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:45">
@@ -2228,112 +2231,112 @@
         <v>1</v>
       </c>
       <c r="J12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="K12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="L12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="M12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="N12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="O12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="P12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="Q12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="R12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="S12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="T12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="U12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="V12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="W12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="X12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="Y12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="Z12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AA12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AB12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AC12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AD12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AE12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AF12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AG12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AH12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AI12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AJ12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AK12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AL12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AM12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AN12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AO12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AP12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AQ12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AR12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
       <c r="AS12">
-        <v>0.963601087</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:45">
@@ -2350,112 +2353,112 @@
         <v>1</v>
       </c>
       <c r="J13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="K13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="L13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="M13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="N13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="O13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="P13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="Q13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="R13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="S13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="T13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="U13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="V13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="W13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="X13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="Y13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="Z13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AA13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AB13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AC13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AD13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AE13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AF13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AG13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AH13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AI13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AJ13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AK13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AL13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AM13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AN13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AO13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AP13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AQ13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AR13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
       <c r="AS13">
-        <v>0.9895587260000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:45">
@@ -2472,112 +2475,112 @@
         <v>1</v>
       </c>
       <c r="J14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="K14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="L14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="M14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="N14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="O14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="P14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="Q14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="R14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="S14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="T14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="U14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="V14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="W14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="X14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="Y14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="Z14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AA14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AB14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AC14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AD14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AE14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AF14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AG14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AH14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AI14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AJ14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AK14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AL14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AM14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AN14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AO14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AP14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AQ14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AR14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
       <c r="AS14">
-        <v>1.017339399</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:45">
@@ -2594,112 +2597,112 @@
         <v>1</v>
       </c>
       <c r="J15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="K15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="L15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="M15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="N15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="O15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="P15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="Q15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="R15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="S15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="T15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="U15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="V15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="W15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="X15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="Y15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="Z15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AA15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AB15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AC15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AD15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AE15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AF15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AG15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AH15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AI15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AJ15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AK15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AL15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AM15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AN15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AO15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AP15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AQ15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AR15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
       <c r="AS15">
-        <v>1.071286848</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:45">
@@ -3326,112 +3329,112 @@
         <v>1</v>
       </c>
       <c r="J21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="K21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="L21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="M21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="N21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="O21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="P21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="Q21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="R21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="S21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="T21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="U21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="V21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="W21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="X21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="Y21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="Z21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AA21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AB21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AC21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AD21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AE21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AF21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AG21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AH21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AI21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AJ21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AK21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AL21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AM21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AN21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AO21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AP21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AQ21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AR21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
       <c r="AS21">
-        <v>0.966884699</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:45">
@@ -3448,112 +3451,112 @@
         <v>1</v>
       </c>
       <c r="J22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="K22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="L22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="M22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="N22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="O22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="P22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="Q22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="R22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="S22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="T22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="U22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="V22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="W22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="X22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="Y22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="Z22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AA22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AB22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AC22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AD22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AE22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AF22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AG22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AH22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AI22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AJ22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AK22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AL22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AM22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AN22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AO22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AP22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AQ22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AR22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
       <c r="AS22">
-        <v>1.012360485</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:45">
@@ -12476,112 +12479,112 @@
         <v>1</v>
       </c>
       <c r="J96">
-        <v>3944281.371</v>
+        <v>3888667.67347042</v>
       </c>
       <c r="K96">
-        <v>3944281.371</v>
+        <v>3831935.04879573</v>
       </c>
       <c r="L96">
-        <v>3944281.371</v>
+        <v>2877043.4682533</v>
       </c>
       <c r="M96">
-        <v>3944281.371</v>
+        <v>2831684.91173217</v>
       </c>
       <c r="N96">
-        <v>3944281.371</v>
+        <v>3149571.80090809</v>
       </c>
       <c r="O96">
-        <v>3944281.371</v>
+        <v>3944281.3714347</v>
       </c>
       <c r="P96">
-        <v>3944281.371</v>
+        <v>3944281</v>
       </c>
       <c r="Q96">
-        <v>3944281.371</v>
+        <v>4784822.26266252</v>
       </c>
       <c r="R96">
-        <v>3944281.371</v>
+        <v>5804486.0610263</v>
       </c>
       <c r="S96">
-        <v>3944281.371</v>
+        <v>7041444.08781042</v>
       </c>
       <c r="T96">
-        <v>3944281.371</v>
+        <v>8542002.568439901</v>
       </c>
       <c r="U96">
-        <v>3944281.371</v>
+        <v>10362335.7608628</v>
       </c>
       <c r="V96">
-        <v>3944281.371</v>
+        <v>12570588.8707626</v>
       </c>
       <c r="W96">
-        <v>3944281.371</v>
+        <v>15249429.1059898</v>
       </c>
       <c r="X96">
-        <v>3944281.371</v>
+        <v>18499140.3703828</v>
       </c>
       <c r="Y96">
-        <v>3944281.371</v>
+        <v>22441377.4485962</v>
       </c>
       <c r="Z96">
-        <v>3944281.371</v>
+        <v>27223720.221976</v>
       </c>
       <c r="AA96">
-        <v>3944281.371</v>
+        <v>33025198.4051356</v>
       </c>
       <c r="AB96">
-        <v>3944281.371</v>
+        <v>40062993.6248811</v>
       </c>
       <c r="AC96">
-        <v>3944281.371</v>
+        <v>48600569.737612</v>
       </c>
       <c r="AD96">
-        <v>3944281.371</v>
+        <v>58957535.7482411</v>
       </c>
       <c r="AE96">
-        <v>3944281.371</v>
+        <v>71521610.5545994</v>
       </c>
       <c r="AF96">
-        <v>3944281.371</v>
+        <v>86763137.42431781</v>
       </c>
       <c r="AG96">
-        <v>3944281.371</v>
+        <v>105252691.561865</v>
       </c>
       <c r="AH96">
-        <v>3944281.371</v>
+        <v>127682439.914997</v>
       </c>
       <c r="AI96">
-        <v>3944281.371</v>
+        <v>154892052.837094</v>
       </c>
       <c r="AJ96">
-        <v>3944281.371</v>
+        <v>187900137.623163</v>
       </c>
       <c r="AK96">
-        <v>3944281.371</v>
+        <v>227942370.651752</v>
       </c>
       <c r="AL96">
-        <v>3944281.371</v>
+        <v>276517755.631146</v>
       </c>
       <c r="AM96">
-        <v>3944281.371</v>
+        <v>335444739.653535</v>
       </c>
       <c r="AN96">
-        <v>3944281.371</v>
+        <v>406929287.793458</v>
       </c>
       <c r="AO96">
-        <v>3944281.371</v>
+        <v>493647464.661757</v>
       </c>
       <c r="AP96">
-        <v>3944281.371</v>
+        <v>598845614.402343</v>
       </c>
       <c r="AQ96">
-        <v>3944281.371</v>
+        <v>726461889.426779</v>
       </c>
       <c r="AR96">
-        <v>3944281.371</v>
+        <v>881273677.3838201</v>
       </c>
       <c r="AS96">
-        <v>3944281.371</v>
+        <v>1069076445.37612</v>
       </c>
     </row>
     <row r="97" spans="1:45">
@@ -12598,112 +12601,112 @@
         <v>1</v>
       </c>
       <c r="J97">
-        <v>391247.6029</v>
+        <v>333566.910296846</v>
       </c>
       <c r="K97">
-        <v>391247.6029</v>
+        <v>390123.440280114</v>
       </c>
       <c r="L97">
-        <v>391247.6029</v>
+        <v>388979.417198126</v>
       </c>
       <c r="M97">
-        <v>391247.6029</v>
+        <v>367934.630600687</v>
       </c>
       <c r="N97">
-        <v>391247.6029</v>
+        <v>373582.35988978</v>
       </c>
       <c r="O97">
-        <v>391247.6029</v>
+        <v>391247.602883924</v>
       </c>
       <c r="P97">
-        <v>391247.6029</v>
+        <v>391247.6</v>
       </c>
       <c r="Q97">
-        <v>391247.6029</v>
+        <v>416121.164644134</v>
       </c>
       <c r="R97">
-        <v>391247.6029</v>
+        <v>442576.066063513</v>
       </c>
       <c r="S97">
-        <v>391247.6029</v>
+        <v>470712.837737454</v>
       </c>
       <c r="T97">
-        <v>391247.6029</v>
+        <v>500638.404560832</v>
       </c>
       <c r="U97">
-        <v>391247.6029</v>
+        <v>532466.489178298</v>
       </c>
       <c r="V97">
-        <v>391247.6029</v>
+        <v>566318.044151189</v>
       </c>
       <c r="W97">
-        <v>391247.6029</v>
+        <v>602321.71159946</v>
       </c>
       <c r="X97">
-        <v>391247.6029</v>
+        <v>640614.312065341</v>
       </c>
       <c r="Y97">
-        <v>391247.6029</v>
+        <v>681341.364456499</v>
       </c>
       <c r="Z97">
-        <v>391247.6029</v>
+        <v>724657.6390445899</v>
       </c>
       <c r="AA97">
-        <v>391247.6029</v>
+        <v>770727.745620685</v>
       </c>
       <c r="AB97">
-        <v>391247.6029</v>
+        <v>819726.759042682</v>
       </c>
       <c r="AC97">
-        <v>391247.6029</v>
+        <v>871840.884551886</v>
       </c>
       <c r="AD97">
-        <v>391247.6029</v>
+        <v>927268.165387093</v>
       </c>
       <c r="AE97">
-        <v>391247.6029</v>
+        <v>986219.235385232</v>
       </c>
       <c r="AF97">
-        <v>391247.6029</v>
+        <v>1048918.11942859</v>
       </c>
       <c r="AG97">
-        <v>391247.6029</v>
+        <v>1115603.08478049</v>
       </c>
       <c r="AH97">
-        <v>391247.6029</v>
+        <v>1186527.54654455</v>
       </c>
       <c r="AI97">
-        <v>391247.6029</v>
+        <v>1261961.03068866</v>
       </c>
       <c r="AJ97">
-        <v>391247.6029</v>
+        <v>1342190.19829305</v>
       </c>
       <c r="AK97">
-        <v>391247.6029</v>
+        <v>1427519.93491499</v>
       </c>
       <c r="AL97">
-        <v>391247.6029</v>
+        <v>1518274.50920988</v>
       </c>
       <c r="AM97">
-        <v>391247.6029</v>
+        <v>1614798.80521163</v>
       </c>
       <c r="AN97">
-        <v>391247.6029</v>
+        <v>1717459.63295524</v>
       </c>
       <c r="AO97">
-        <v>391247.6029</v>
+        <v>1826647.12242228</v>
       </c>
       <c r="AP97">
-        <v>391247.6029</v>
+        <v>1942776.20610635</v>
       </c>
       <c r="AQ97">
-        <v>391247.6029</v>
+        <v>2066288.19583274</v>
       </c>
       <c r="AR97">
-        <v>391247.6029</v>
+        <v>2197652.45982428</v>
       </c>
       <c r="AS97">
-        <v>391247.6029</v>
+        <v>2337368.20638676</v>
       </c>
     </row>
     <row r="98" spans="1:45">
@@ -12720,112 +12723,112 @@
         <v>1</v>
       </c>
       <c r="J98">
-        <v>193163.7998</v>
+        <v>239717.501040869</v>
       </c>
       <c r="K98">
-        <v>193163.7998</v>
+        <v>241472.131523638</v>
       </c>
       <c r="L98">
-        <v>193163.7998</v>
+        <v>228084.76129832</v>
       </c>
       <c r="M98">
-        <v>193163.7998</v>
+        <v>201777.556029345</v>
       </c>
       <c r="N98">
-        <v>193163.7998</v>
+        <v>207193.494628157</v>
       </c>
       <c r="O98">
-        <v>193163.7998</v>
+        <v>193163.799825183</v>
       </c>
       <c r="P98">
-        <v>193163.7998</v>
+        <v>193163.8</v>
       </c>
       <c r="Q98">
-        <v>193163.7998</v>
+        <v>198954.851882983</v>
       </c>
       <c r="R98">
-        <v>193163.7998</v>
+        <v>204919.519536164</v>
       </c>
       <c r="S98">
-        <v>193163.7998</v>
+        <v>211063.007961375</v>
       </c>
       <c r="T98">
-        <v>193163.7998</v>
+        <v>217390.678206435</v>
       </c>
       <c r="U98">
-        <v>193163.7998</v>
+        <v>223908.052043408</v>
       </c>
       <c r="V98">
-        <v>193163.7998</v>
+        <v>230620.816787118</v>
       </c>
       <c r="W98">
-        <v>193163.7998</v>
+        <v>237534.83025812</v>
       </c>
       <c r="X98">
-        <v>193163.7998</v>
+        <v>244656.125894468</v>
       </c>
       <c r="Y98">
-        <v>193163.7998</v>
+        <v>251990.918016721</v>
       </c>
       <c r="Z98">
-        <v>193163.7998</v>
+        <v>259545.607250807</v>
       </c>
       <c r="AA98">
-        <v>193163.7998</v>
+        <v>267326.78611346</v>
       </c>
       <c r="AB98">
-        <v>193163.7998</v>
+        <v>275341.244765103</v>
       </c>
       <c r="AC98">
-        <v>193163.7998</v>
+        <v>283595.976935208</v>
       </c>
       <c r="AD98">
-        <v>193163.7998</v>
+        <v>292098.186025301</v>
       </c>
       <c r="AE98">
-        <v>193163.7998</v>
+        <v>300855.291394929</v>
       </c>
       <c r="AF98">
-        <v>193163.7998</v>
+        <v>309874.93483608</v>
       </c>
       <c r="AG98">
-        <v>193163.7998</v>
+        <v>319164.987241716</v>
       </c>
       <c r="AH98">
-        <v>193163.7998</v>
+        <v>328733.555474212</v>
       </c>
       <c r="AI98">
-        <v>193163.7998</v>
+        <v>338588.989439731</v>
       </c>
       <c r="AJ98">
-        <v>193163.7998</v>
+        <v>348739.889374668</v>
       </c>
       <c r="AK98">
-        <v>193163.7998</v>
+        <v>359195.113350559</v>
       </c>
       <c r="AL98">
-        <v>193163.7998</v>
+        <v>369963.78500398</v>
       </c>
       <c r="AM98">
-        <v>193163.7998</v>
+        <v>381055.301498182</v>
       </c>
       <c r="AN98">
-        <v>193163.7998</v>
+        <v>392479.341723429</v>
       </c>
       <c r="AO98">
-        <v>193163.7998</v>
+        <v>404245.874743174</v>
       </c>
       <c r="AP98">
-        <v>193163.7998</v>
+        <v>416365.168493449</v>
       </c>
       <c r="AQ98">
-        <v>193163.7998</v>
+        <v>428847.798743074</v>
       </c>
       <c r="AR98">
-        <v>193163.7998</v>
+        <v>441704.658322478</v>
       </c>
       <c r="AS98">
-        <v>193163.7998</v>
+        <v>454946.966629214</v>
       </c>
     </row>
     <row r="99" spans="1:45">
@@ -12842,112 +12845,112 @@
         <v>1</v>
       </c>
       <c r="J99">
-        <v>29174.73605</v>
+        <v>27606.9711441172</v>
       </c>
       <c r="K99">
-        <v>29174.73605</v>
+        <v>32382.0506228358</v>
       </c>
       <c r="L99">
-        <v>29174.73605</v>
+        <v>36564.3631069558</v>
       </c>
       <c r="M99">
-        <v>29174.73605</v>
+        <v>36960.8294622997</v>
       </c>
       <c r="N99">
-        <v>29174.73605</v>
+        <v>33601.2696173966</v>
       </c>
       <c r="O99">
-        <v>29174.73605</v>
+        <v>29174.7360464457</v>
       </c>
       <c r="P99">
-        <v>29174.73605</v>
+        <v>29174.74</v>
       </c>
       <c r="Q99">
-        <v>29174.73605</v>
+        <v>30442.2004317971</v>
       </c>
       <c r="R99">
-        <v>29174.73605</v>
+        <v>31764.7241116702</v>
       </c>
       <c r="S99">
-        <v>29174.73605</v>
+        <v>33144.7031942086</v>
       </c>
       <c r="T99">
-        <v>29174.73605</v>
+        <v>34584.6337581937</v>
       </c>
       <c r="U99">
-        <v>29174.73605</v>
+        <v>36087.1203214572</v>
       </c>
       <c r="V99">
-        <v>29174.73605</v>
+        <v>37654.8805518808</v>
       </c>
       <c r="W99">
-        <v>29174.73605</v>
+        <v>39290.7501830603</v>
       </c>
       <c r="X99">
-        <v>29174.73605</v>
+        <v>40997.6881435239</v>
       </c>
       <c r="Y99">
-        <v>29174.73605</v>
+        <v>42778.7819087837</v>
       </c>
       <c r="Z99">
-        <v>29174.73605</v>
+        <v>44637.2530859</v>
       </c>
       <c r="AA99">
-        <v>29174.73605</v>
+        <v>46576.4632406603</v>
       </c>
       <c r="AB99">
-        <v>29174.73605</v>
+        <v>48599.9199779129</v>
       </c>
       <c r="AC99">
-        <v>29174.73605</v>
+        <v>50711.2832860525</v>
       </c>
       <c r="AD99">
-        <v>29174.73605</v>
+        <v>52914.372157135</v>
       </c>
       <c r="AE99">
-        <v>29174.73605</v>
+        <v>55213.1714945946</v>
       </c>
       <c r="AF99">
-        <v>29174.73605</v>
+        <v>57611.8393210578</v>
       </c>
       <c r="AG99">
-        <v>29174.73605</v>
+        <v>60114.7142992923</v>
       </c>
       <c r="AH99">
-        <v>29174.73605</v>
+        <v>62726.323579894</v>
       </c>
       <c r="AI99">
-        <v>29174.73605</v>
+        <v>65451.3909899076</v>
       </c>
       <c r="AJ99">
-        <v>29174.73605</v>
+        <v>68294.8455771907</v>
       </c>
       <c r="AK99">
-        <v>29174.73605</v>
+        <v>71261.8305259781</v>
       </c>
       <c r="AL99">
-        <v>29174.73605</v>
+        <v>74357.7124597712</v>
       </c>
       <c r="AM99">
-        <v>29174.73605</v>
+        <v>77588.0911483802</v>
       </c>
       <c r="AN99">
-        <v>29174.73605</v>
+        <v>80958.8096366766</v>
       </c>
       <c r="AO99">
-        <v>29174.73605</v>
+        <v>84475.96481337689</v>
       </c>
       <c r="AP99">
-        <v>29174.73605</v>
+        <v>88145.91843897371</v>
       </c>
       <c r="AQ99">
-        <v>29174.73605</v>
+        <v>91975.3086527619</v>
       </c>
       <c r="AR99">
-        <v>29174.73605</v>
+        <v>95971.0619797738</v>
       </c>
       <c r="AS99">
-        <v>29174.73605</v>
+        <v>100140.405859339</v>
       </c>
     </row>
     <row r="100" spans="1:45">
@@ -12964,112 +12967,112 @@
         <v>1</v>
       </c>
       <c r="J100">
-        <v>4136.366244</v>
+        <v>18885.1010776033</v>
       </c>
       <c r="K100">
-        <v>4136.366244</v>
+        <v>30307.2741946805</v>
       </c>
       <c r="L100">
-        <v>4136.366244</v>
+        <v>895.17785011236</v>
       </c>
       <c r="M100">
-        <v>4136.366244</v>
+        <v>3113.11545284935</v>
       </c>
       <c r="N100">
-        <v>4136.366244</v>
+        <v>0</v>
       </c>
       <c r="O100">
-        <v>4136.366244</v>
+        <v>4136.36624444119</v>
       </c>
       <c r="P100">
-        <v>4136.366244</v>
-      </c>
-      <c r="Q100">
-        <v>4136.366244</v>
-      </c>
-      <c r="R100">
-        <v>4136.366244</v>
-      </c>
-      <c r="S100">
-        <v>4136.366244</v>
-      </c>
-      <c r="T100">
-        <v>4136.366244</v>
-      </c>
-      <c r="U100">
-        <v>4136.366244</v>
-      </c>
-      <c r="V100">
-        <v>4136.366244</v>
-      </c>
-      <c r="W100">
-        <v>4136.366244</v>
-      </c>
-      <c r="X100">
-        <v>4136.366244</v>
-      </c>
-      <c r="Y100">
-        <v>4136.366244</v>
-      </c>
-      <c r="Z100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AA100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AB100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AC100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AD100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AE100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AF100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AG100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AH100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AI100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AJ100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AK100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AL100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AM100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AN100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AO100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AP100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AQ100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AR100">
-        <v>4136.366244</v>
-      </c>
-      <c r="AS100">
-        <v>4136.366244</v>
+        <v>4136.366</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>160</v>
+      </c>
+      <c r="R100" t="s">
+        <v>160</v>
+      </c>
+      <c r="S100" t="s">
+        <v>160</v>
+      </c>
+      <c r="T100" t="s">
+        <v>160</v>
+      </c>
+      <c r="U100" t="s">
+        <v>160</v>
+      </c>
+      <c r="V100" t="s">
+        <v>160</v>
+      </c>
+      <c r="W100" t="s">
+        <v>160</v>
+      </c>
+      <c r="X100" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y100" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AC100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AD100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AG100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AI100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AJ100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AK100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AL100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AM100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AN100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AQ100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AR100" t="s">
+        <v>160</v>
+      </c>
+      <c r="AS100" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="101" spans="1:45">
@@ -13086,112 +13089,112 @@
         <v>1</v>
       </c>
       <c r="J101">
-        <v>1660792.974</v>
+        <v>1553788.81741633</v>
       </c>
       <c r="K101">
-        <v>1660792.974</v>
+        <v>1517605.80694588</v>
       </c>
       <c r="L101">
-        <v>1660792.974</v>
+        <v>1779877.12595883</v>
       </c>
       <c r="M101">
-        <v>1660792.974</v>
+        <v>1808668.34563003</v>
       </c>
       <c r="N101">
-        <v>1660792.974</v>
+        <v>1786240.34372464</v>
       </c>
       <c r="O101">
-        <v>1660792.974</v>
+        <v>1660792.97436594</v>
       </c>
       <c r="P101">
-        <v>1660792.974</v>
+        <v>1660793</v>
       </c>
       <c r="Q101">
-        <v>1660792.974</v>
+        <v>1753082.17420821</v>
       </c>
       <c r="R101">
-        <v>1660792.974</v>
+        <v>1850499.79710089</v>
       </c>
       <c r="S101">
-        <v>1660792.974</v>
+        <v>1953330.85319692</v>
       </c>
       <c r="T101">
-        <v>1660792.974</v>
+        <v>2061876.16341737</v>
       </c>
       <c r="U101">
-        <v>1660792.974</v>
+        <v>2176453.26510395</v>
       </c>
       <c r="V101">
-        <v>1660792.974</v>
+        <v>2297397.34093953</v>
       </c>
       <c r="W101">
-        <v>1660792.974</v>
+        <v>2425062.19948809</v>
       </c>
       <c r="X101">
-        <v>1660792.974</v>
+        <v>2559821.31022272</v>
       </c>
       <c r="Y101">
-        <v>1660792.974</v>
+        <v>2702068.89606937</v>
       </c>
       <c r="Z101">
-        <v>1660792.974</v>
+        <v>2852221.08666262</v>
       </c>
       <c r="AA101">
-        <v>1660792.974</v>
+        <v>3010717.13568698</v>
       </c>
       <c r="AB101">
-        <v>1660792.974</v>
+        <v>3178020.70586523</v>
       </c>
       <c r="AC101">
-        <v>1660792.974</v>
+        <v>3354621.22535254</v>
       </c>
       <c r="AD101">
-        <v>1660792.974</v>
+        <v>3541035.31950461</v>
       </c>
       <c r="AE101">
-        <v>1660792.974</v>
+        <v>3737808.32220825</v>
       </c>
       <c r="AF101">
-        <v>1660792.974</v>
+        <v>3945515.87119548</v>
       </c>
       <c r="AG101">
-        <v>1660792.974</v>
+        <v>4164765.59200837</v>
       </c>
       <c r="AH101">
-        <v>1660792.974</v>
+        <v>4396198.87554052</v>
       </c>
       <c r="AI101">
-        <v>1660792.974</v>
+        <v>4640492.75435544</v>
       </c>
       <c r="AJ101">
-        <v>1660792.974</v>
+        <v>4898361.88327074</v>
       </c>
       <c r="AK101">
-        <v>1660792.974</v>
+        <v>5170560.63000198</v>
       </c>
       <c r="AL101">
-        <v>1660792.974</v>
+        <v>5457885.2819823</v>
       </c>
       <c r="AM101">
-        <v>1660792.974</v>
+        <v>5761176.37581354</v>
       </c>
       <c r="AN101">
-        <v>1660792.974</v>
+        <v>6081321.15616344</v>
       </c>
       <c r="AO101">
-        <v>1660792.974</v>
+        <v>6419256.17130212</v>
       </c>
       <c r="AP101">
-        <v>1660792.974</v>
+        <v>6775970.01287082</v>
       </c>
       <c r="AQ101">
-        <v>1660792.974</v>
+        <v>7152506.20789779</v>
       </c>
       <c r="AR101">
-        <v>1660792.974</v>
+        <v>7549966.27152158</v>
       </c>
       <c r="AS101">
-        <v>1660792.974</v>
+        <v>7969512.92935223</v>
       </c>
     </row>
     <row r="102" spans="1:45">
@@ -13330,112 +13333,112 @@
         <v>1</v>
       </c>
       <c r="J103">
-        <v>803025.1581999999</v>
+        <v>889229.42265422</v>
       </c>
       <c r="K103">
-        <v>803025.1581999999</v>
+        <v>931730.151395607</v>
       </c>
       <c r="L103">
-        <v>803025.1581999999</v>
+        <v>1007907.72808513</v>
       </c>
       <c r="M103">
-        <v>803025.1581999999</v>
+        <v>1009731.64765887</v>
       </c>
       <c r="N103">
-        <v>803025.1581999999</v>
+        <v>856697.039245791</v>
       </c>
       <c r="O103">
-        <v>803025.1581999999</v>
+        <v>803025.158244407</v>
       </c>
       <c r="P103">
-        <v>803025.1581999999</v>
+        <v>803025.2</v>
       </c>
       <c r="Q103">
-        <v>803025.1581999999</v>
+        <v>827427.0559927321</v>
       </c>
       <c r="R103">
-        <v>803025.1581999999</v>
+        <v>852570.421188276</v>
       </c>
       <c r="S103">
-        <v>803025.1581999999</v>
+        <v>878477.828130797</v>
       </c>
       <c r="T103">
-        <v>803025.1581999999</v>
+        <v>905172.494070117</v>
       </c>
       <c r="U103">
-        <v>803025.1581999999</v>
+        <v>932678.341768148</v>
       </c>
       <c r="V103">
-        <v>803025.1581999999</v>
+        <v>961020.020937576</v>
       </c>
       <c r="W103">
-        <v>803025.1581999999</v>
+        <v>990222.930332015</v>
       </c>
       <c r="X103">
-        <v>803025.1581999999</v>
+        <v>1020313.24050742</v>
       </c>
       <c r="Y103">
-        <v>803025.1581999999</v>
+        <v>1051317.91727514</v>
       </c>
       <c r="Z103">
-        <v>803025.1581999999</v>
+        <v>1083264.74586773</v>
       </c>
       <c r="AA103">
-        <v>803025.1581999999</v>
+        <v>1116182.35583896</v>
       </c>
       <c r="AB103">
-        <v>803025.1581999999</v>
+        <v>1150100.2467206</v>
       </c>
       <c r="AC103">
-        <v>803025.1581999999</v>
+        <v>1185048.8144588</v>
       </c>
       <c r="AD103">
-        <v>803025.1581999999</v>
+        <v>1221059.37865377</v>
       </c>
       <c r="AE103">
-        <v>803025.1581999999</v>
+        <v>1258164.21062727</v>
       </c>
       <c r="AF103">
-        <v>803025.1581999999</v>
+        <v>1296396.56234293</v>
       </c>
       <c r="AG103">
-        <v>803025.1581999999</v>
+        <v>1335790.69620543</v>
       </c>
       <c r="AH103">
-        <v>803025.1581999999</v>
+        <v>1376381.91576521</v>
       </c>
       <c r="AI103">
-        <v>803025.1581999999</v>
+        <v>1418206.59735616</v>
       </c>
       <c r="AJ103">
-        <v>803025.1581999999</v>
+        <v>1461302.22269472</v>
       </c>
       <c r="AK103">
-        <v>803025.1581999999</v>
+        <v>1505707.41246966</v>
       </c>
       <c r="AL103">
-        <v>803025.1581999999</v>
+        <v>1551461.96095241</v>
       </c>
       <c r="AM103">
-        <v>803025.1581999999</v>
+        <v>1598606.87165928</v>
       </c>
       <c r="AN103">
-        <v>803025.1581999999</v>
+        <v>1647184.39409721</v>
       </c>
       <c r="AO103">
-        <v>803025.1581999999</v>
+        <v>1697238.06162624</v>
       </c>
       <c r="AP103">
-        <v>803025.1581999999</v>
+        <v>1748812.73047248</v>
       </c>
       <c r="AQ103">
-        <v>803025.1581999999</v>
+        <v>1801954.61992657</v>
       </c>
       <c r="AR103">
-        <v>803025.1581999999</v>
+        <v>1856711.35376367</v>
       </c>
       <c r="AS103">
-        <v>803025.1581999999</v>
+        <v>1913132.00292214</v>
       </c>
     </row>
     <row r="104" spans="1:45">
@@ -13452,112 +13455,112 @@
         <v>1</v>
       </c>
       <c r="J104">
-        <v>386455.3512</v>
+        <v>408522.402065329</v>
       </c>
       <c r="K104">
-        <v>386455.3512</v>
+        <v>436587.643264139</v>
       </c>
       <c r="L104">
-        <v>386455.3512</v>
+        <v>434947.903497555</v>
       </c>
       <c r="M104">
-        <v>386455.3512</v>
+        <v>452552.949343296</v>
       </c>
       <c r="N104">
-        <v>386455.3512</v>
+        <v>424190.452460617</v>
       </c>
       <c r="O104">
-        <v>386455.3512</v>
+        <v>386455.35119185</v>
       </c>
       <c r="P104">
-        <v>386455.3512</v>
+        <v>386455.4</v>
       </c>
       <c r="Q104">
-        <v>386455.3512</v>
+        <v>403588.961914573</v>
       </c>
       <c r="R104">
-        <v>386455.3512</v>
+        <v>421482.143034572</v>
       </c>
       <c r="S104">
-        <v>386455.3512</v>
+        <v>440168.621198856</v>
       </c>
       <c r="T104">
-        <v>386455.3512</v>
+        <v>459683.567358653</v>
       </c>
       <c r="U104">
-        <v>386455.3512</v>
+        <v>480063.711774933</v>
       </c>
       <c r="V104">
-        <v>386455.3512</v>
+        <v>501347.413150655</v>
       </c>
       <c r="W104">
-        <v>386455.3512</v>
+        <v>523574.730828006</v>
       </c>
       <c r="X104">
-        <v>386455.3512</v>
+        <v>546787.5001865081</v>
       </c>
       <c r="Y104">
-        <v>386455.3512</v>
+        <v>571029.411383919</v>
       </c>
       <c r="Z104">
-        <v>386455.3512</v>
+        <v>596346.091588125</v>
       </c>
       <c r="AA104">
-        <v>386455.3512</v>
+        <v>622785.19085479</v>
       </c>
       <c r="AB104">
-        <v>386455.3512</v>
+        <v>650396.47181241</v>
       </c>
       <c r="AC104">
-        <v>386455.3512</v>
+        <v>679231.90332357</v>
       </c>
       <c r="AD104">
-        <v>386455.3512</v>
+        <v>709345.758298678</v>
       </c>
       <c r="AE104">
-        <v>386455.3512</v>
+        <v>740794.715846302</v>
       </c>
       <c r="AF104">
-        <v>386455.3512</v>
+        <v>773637.967952344</v>
       </c>
       <c r="AG104">
-        <v>386455.3512</v>
+        <v>807937.3308888579</v>
       </c>
       <c r="AH104">
-        <v>386455.3512</v>
+        <v>843757.3615622011</v>
       </c>
       <c r="AI104">
-        <v>386455.3512</v>
+        <v>881165.479019487</v>
       </c>
       <c r="AJ104">
-        <v>386455.3512</v>
+        <v>920232.09134206</v>
       </c>
       <c r="AK104">
-        <v>386455.3512</v>
+        <v>961030.728164798</v>
       </c>
       <c r="AL104">
-        <v>386455.3512</v>
+        <v>1003638.17907069</v>
       </c>
       <c r="AM104">
-        <v>386455.3512</v>
+        <v>1048134.63812118</v>
       </c>
       <c r="AN104">
-        <v>386455.3512</v>
+        <v>1094603.85479419</v>
       </c>
       <c r="AO104">
-        <v>386455.3512</v>
+        <v>1143133.29161419</v>
       </c>
       <c r="AP104">
-        <v>386455.3512</v>
+        <v>1193814.2887706</v>
       </c>
       <c r="AQ104">
-        <v>386455.3512</v>
+        <v>1246742.23603477</v>
       </c>
       <c r="AR104">
-        <v>386455.3512</v>
+        <v>1302016.75229878</v>
       </c>
       <c r="AS104">
-        <v>386455.3512</v>
+        <v>1359741.87307423</v>
       </c>
     </row>
     <row r="105" spans="1:45">
@@ -14306,112 +14309,112 @@
         <v>1</v>
       </c>
       <c r="J111">
-        <v>13449.72472</v>
+        <v>13704.5313164684</v>
       </c>
       <c r="K111">
-        <v>13449.72472</v>
+        <v>13481.8438884558</v>
       </c>
       <c r="L111">
-        <v>13449.72472</v>
+        <v>14839.0919685393</v>
       </c>
       <c r="M111">
-        <v>13449.72472</v>
+        <v>13936.4180000342</v>
       </c>
       <c r="N111">
-        <v>13449.72472</v>
+        <v>13957.1434283665</v>
       </c>
       <c r="O111">
-        <v>13449.72472</v>
+        <v>13449.7247197699</v>
       </c>
       <c r="P111">
-        <v>13449.72472</v>
+        <v>13449.72</v>
       </c>
       <c r="Q111">
-        <v>13449.72472</v>
+        <v>13824.7221811756</v>
       </c>
       <c r="R111">
-        <v>13449.72472</v>
+        <v>14210.1800919788</v>
       </c>
       <c r="S111">
-        <v>13449.72472</v>
+        <v>14606.3852567994</v>
       </c>
       <c r="T111">
-        <v>13449.72472</v>
+        <v>15013.637328247</v>
       </c>
       <c r="U111">
-        <v>13449.72472</v>
+        <v>15432.2443137807</v>
       </c>
       <c r="V111">
-        <v>13449.72472</v>
+        <v>15862.5228086567</v>
       </c>
       <c r="W111">
-        <v>13449.72472</v>
+        <v>16304.7982353715</v>
       </c>
       <c r="X111">
-        <v>13449.72472</v>
+        <v>16759.4050897813</v>
       </c>
       <c r="Y111">
-        <v>13449.72472</v>
+        <v>17226.6871940834</v>
       </c>
       <c r="Z111">
-        <v>13449.72472</v>
+        <v>17706.997956851</v>
       </c>
       <c r="AA111">
-        <v>13449.72472</v>
+        <v>18200.7006403189</v>
       </c>
       <c r="AB111">
-        <v>13449.72472</v>
+        <v>18708.1686351206</v>
       </c>
       <c r="AC111">
-        <v>13449.72472</v>
+        <v>19229.7857426865</v>
       </c>
       <c r="AD111">
-        <v>13449.72472</v>
+        <v>19765.9464655155</v>
       </c>
       <c r="AE111">
-        <v>13449.72472</v>
+        <v>20317.0563055395</v>
       </c>
       <c r="AF111">
-        <v>13449.72472</v>
+        <v>20883.5320708079</v>
       </c>
       <c r="AG111">
-        <v>13449.72472</v>
+        <v>21465.8021907215</v>
       </c>
       <c r="AH111">
-        <v>13449.72472</v>
+        <v>22064.307040057</v>
       </c>
       <c r="AI111">
-        <v>13449.72472</v>
+        <v>22679.4992720254</v>
       </c>
       <c r="AJ111">
-        <v>13449.72472</v>
+        <v>23311.8441606164</v>
       </c>
       <c r="AK111">
-        <v>13449.72472</v>
+        <v>23961.8199524885</v>
       </c>
       <c r="AL111">
-        <v>13449.72472</v>
+        <v>24629.9182286697</v>
       </c>
       <c r="AM111">
-        <v>13449.72472</v>
+        <v>25316.6442763442</v>
       </c>
       <c r="AN111">
-        <v>13449.72472</v>
+        <v>26022.5174710037</v>
       </c>
       <c r="AO111">
-        <v>13449.72472</v>
+        <v>26748.0716692552</v>
       </c>
       <c r="AP111">
-        <v>13449.72472</v>
+        <v>27493.8556125799</v>
       </c>
       <c r="AQ111">
-        <v>13449.72472</v>
+        <v>28260.4333423501</v>
       </c>
       <c r="AR111">
-        <v>13449.72472</v>
+        <v>29048.3846264177</v>
       </c>
       <c r="AS111">
-        <v>13449.72472</v>
+        <v>29858.3053975962</v>
       </c>
     </row>
     <row r="112" spans="1:45">
@@ -14428,112 +14431,112 @@
         <v>1</v>
       </c>
       <c r="J112">
-        <v>55827.44077</v>
+        <v>57431.5870717435</v>
       </c>
       <c r="K112">
-        <v>55827.44077</v>
+        <v>55052.5025622209</v>
       </c>
       <c r="L112">
-        <v>55827.44077</v>
+        <v>58961.2844577723</v>
       </c>
       <c r="M112">
-        <v>55827.44077</v>
+        <v>58982.6522304586</v>
       </c>
       <c r="N112">
-        <v>55827.44077</v>
+        <v>56960.9014802083</v>
       </c>
       <c r="O112">
-        <v>55827.44077</v>
+        <v>55827.4407667426</v>
       </c>
       <c r="P112">
-        <v>55827.44077</v>
+        <v>55827.44</v>
       </c>
       <c r="Q112">
-        <v>55827.44077</v>
+        <v>57387.8631731203</v>
       </c>
       <c r="R112">
-        <v>55827.44077</v>
+        <v>58991.9014659597</v>
       </c>
       <c r="S112">
-        <v>55827.44077</v>
+        <v>60640.7739572277</v>
       </c>
       <c r="T112">
-        <v>55827.44077</v>
+        <v>62335.7337998931</v>
       </c>
       <c r="U112">
-        <v>55827.44077</v>
+        <v>64078.0691735877</v>
       </c>
       <c r="V112">
-        <v>55827.44077</v>
+        <v>65869.1042636308</v>
       </c>
       <c r="W112">
-        <v>55827.44077</v>
+        <v>67710.2002674176</v>
       </c>
       <c r="X112">
-        <v>55827.44077</v>
+        <v>69602.7564289377</v>
       </c>
       <c r="Y112">
-        <v>55827.44077</v>
+        <v>71548.21110220889</v>
       </c>
       <c r="Z112">
-        <v>55827.44077</v>
+        <v>73548.0428444344</v>
       </c>
       <c r="AA112">
-        <v>55827.44077</v>
+        <v>75603.7715397158</v>
       </c>
       <c r="AB112">
-        <v>55827.44077</v>
+        <v>77716.95955417371</v>
       </c>
       <c r="AC112">
-        <v>55827.44077</v>
+        <v>79889.2129233553</v>
       </c>
       <c r="AD112">
-        <v>55827.44077</v>
+        <v>82122.1825728314</v>
       </c>
       <c r="AE112">
-        <v>55827.44077</v>
+        <v>84417.5655729092</v>
       </c>
       <c r="AF112">
-        <v>55827.44077</v>
+        <v>86777.1064284164</v>
       </c>
       <c r="AG112">
-        <v>55827.44077</v>
+        <v>89202.5984045347</v>
       </c>
       <c r="AH112">
-        <v>55827.44077</v>
+        <v>91695.884889693</v>
       </c>
       <c r="AI112">
-        <v>55827.44077</v>
+        <v>94258.8607965526</v>
       </c>
       <c r="AJ112">
-        <v>55827.44077</v>
+        <v>96893.474002153</v>
       </c>
       <c r="AK112">
-        <v>55827.44077</v>
+        <v>99601.72682830961</v>
       </c>
       <c r="AL112">
-        <v>55827.44077</v>
+        <v>102385.677563391</v>
       </c>
       <c r="AM112">
-        <v>55827.44077</v>
+        <v>105247.442026628</v>
       </c>
       <c r="AN112">
-        <v>55827.44077</v>
+        <v>108189.195176155</v>
       </c>
       <c r="AO112">
-        <v>55827.44077</v>
+        <v>111213.172761982</v>
       </c>
       <c r="AP112">
-        <v>55827.44077</v>
+        <v>114321.673025186</v>
       </c>
       <c r="AQ112">
-        <v>55827.44077</v>
+        <v>117517.058444586</v>
       </c>
       <c r="AR112">
-        <v>55827.44077</v>
+        <v>120801.757532236</v>
       </c>
       <c r="AS112">
-        <v>55827.44077</v>
+        <v>124178.266679117</v>
       </c>
     </row>
     <row r="113" spans="1:45">

</xml_diff>